<commit_message>
Results - second part
</commit_message>
<xml_diff>
--- a/HTML-CSS/Test/Test-HTML-CSS.xlsx
+++ b/HTML-CSS/Test/Test-HTML-CSS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dženan Košuta\GitHub\IT Camp - 2. grupa\HTML-CSS\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD06BE04-1C41-4D21-8E85-01BBF987EE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C38159-DB75-4EBA-BB58-1CBCBD8712BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,7 +544,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,12 +626,18 @@
       <c r="C5" s="2">
         <v>28</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="3">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3">
+        <v>19</v>
+      </c>
       <c r="G5" s="4">
         <f t="shared" ref="G5:G19" si="0">C5+D5+E5+F5</f>
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -710,12 +716,18 @@
       <c r="C9" s="2">
         <v>28</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="3">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5">
+        <v>28</v>
+      </c>
+      <c r="F9" s="3">
+        <v>19</v>
+      </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -746,12 +758,18 @@
       <c r="C11" s="2">
         <v>23</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3"/>
+      <c r="D11" s="3">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3">
+        <v>20</v>
+      </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -788,12 +806,18 @@
       <c r="C13" s="2">
         <v>20</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="3">
+        <v>18</v>
+      </c>
+      <c r="E13" s="5">
+        <v>26</v>
+      </c>
+      <c r="F13" s="3">
+        <v>14</v>
+      </c>
       <c r="G13" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -806,12 +830,18 @@
       <c r="C14" s="2">
         <v>27</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
+      <c r="D14" s="3">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3">
+        <v>19</v>
+      </c>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -848,12 +878,18 @@
       <c r="C16" s="2">
         <v>27</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="3"/>
+      <c r="D16" s="3">
+        <v>20</v>
+      </c>
+      <c r="E16" s="5">
+        <v>26</v>
+      </c>
+      <c r="F16" s="3">
+        <v>20</v>
+      </c>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
One more result for test
</commit_message>
<xml_diff>
--- a/HTML-CSS/Test/Test-HTML-CSS.xlsx
+++ b/HTML-CSS/Test/Test-HTML-CSS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dženan Košuta\GitHub\IT Camp - 2. grupa\HTML-CSS\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C988CF-4703-40F2-AEDA-E06198FF4A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218E79BE-F1E6-4BF0-B7C0-EF7ECE85EA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>TEST</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Hasan Mujanović</t>
+  </si>
+  <si>
+    <t>Amir Zornić</t>
   </si>
 </sst>
 </file>
@@ -541,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -642,7 +645,7 @@
         <v>19</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G19" si="0">C5+D5+E5+F5</f>
+        <f t="shared" ref="G5:G20" si="0">C5+D5+E5+F5</f>
         <v>88</v>
       </c>
     </row>
@@ -963,21 +966,45 @@
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3">
+        <v>20</v>
+      </c>
+      <c r="E19" s="5">
+        <v>30</v>
+      </c>
+      <c r="F19" s="3">
+        <v>20</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="2">
-        <v>30</v>
-      </c>
-      <c r="D19" s="3">
-        <v>20</v>
-      </c>
-      <c r="E19" s="5">
+      <c r="C20" s="2">
+        <v>30</v>
+      </c>
+      <c r="D20" s="3">
+        <v>20</v>
+      </c>
+      <c r="E20" s="5">
         <v>27</v>
       </c>
-      <c r="F19" s="3">
-        <v>20</v>
-      </c>
-      <c r="G19" s="4">
+      <c r="F20" s="3">
+        <v>20</v>
+      </c>
+      <c r="G20" s="4">
         <f t="shared" si="0"/>
         <v>97</v>
       </c>

</xml_diff>